<commit_message>
ExcelDocumentReader tests and fix
</commit_message>
<xml_diff>
--- a/src/main/resources/excelsheets/TestData.xlsx
+++ b/src/main/resources/excelsheets/TestData.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\git\Orasi-Selenium-Java-Core\src\main\resources\excelsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\git\Selenium-Java-Core\src\main\resources\excelsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="18200" windowHeight="6980"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="18195" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Column1</t>
   </si>
@@ -55,36 +55,12 @@
   </si>
   <si>
     <t>lmno</t>
-  </si>
-  <si>
-    <t>pqrs</t>
-  </si>
-  <si>
-    <t>tuvz</t>
-  </si>
-  <si>
-    <t>xyz0</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>5678</t>
-  </si>
-  <si>
-    <t>9012</t>
-  </si>
-  <si>
-    <t>3456</t>
-  </si>
-  <si>
-    <t>7890</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -563,9 +539,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -700,6 +677,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -735,6 +729,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -917,9 +928,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -936,7 +947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -953,39 +964,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <f>IF(,D4=E4)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>SUM(12,23)</f>
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B4" s="2">
+        <v>5678</v>
+      </c>
+      <c r="C4" s="2">
+        <v>9012</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3456</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>